<commit_message>
feat: super excel 3.0
</commit_message>
<xml_diff>
--- a/9.1B - 3.xlsx
+++ b/9.1B - 3.xlsx
@@ -8,72 +8,131 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Desktop\trabalhoPO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39EC1EA-9C14-4291-B7D0-687E8A031B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB45AF4-A493-4201-B0A9-005F5BCB11F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" 9.1B - 3" sheetId="3" r:id="rId1"/>
+    <sheet name=" 9.1B - 3 2.0" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">' 9.1B - 3'!$B$8:$G$8</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!$B$8:$G$8</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">' 9.1B - 3'!$B$8:$G$8</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!$B$8:$G$8</definedName>
     <definedName name="solver_lhs10" localSheetId="0" hidden="1">' 9.1B - 3'!#REF!</definedName>
+    <definedName name="solver_lhs10" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!#REF!</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">' 9.1B - 3'!$H$2:$H$7</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!$H$2:$H$7</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">' 9.1B - 3'!$J$4</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!$J$4</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">' 9.1B - 3'!$J$6</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!$J$6</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">' 9.1B - 3'!#REF!</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!#REF!</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">' 9.1B - 3'!#REF!</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!#REF!</definedName>
     <definedName name="solver_lhs7" localSheetId="0" hidden="1">' 9.1B - 3'!$J$6</definedName>
+    <definedName name="solver_lhs7" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!$J$6</definedName>
     <definedName name="solver_lhs8" localSheetId="0" hidden="1">' 9.1B - 3'!$H$14</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!$H$14</definedName>
     <definedName name="solver_lhs9" localSheetId="0" hidden="1">' 9.1B - 3'!$I$11</definedName>
+    <definedName name="solver_lhs9" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!$I$11</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">' 9.1B - 3'!$J$8</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!$J$8</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">5</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_rel10" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel10" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel7" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel7" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel8" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel9" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">"binário"</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">"binário"</definedName>
     <definedName name="solver_rhs10" localSheetId="0" hidden="1">' 9.1B - 3'!#REF!</definedName>
+    <definedName name="solver_rhs10" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!#REF!</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">' 9.1B - 3'!$J$2:$J$7</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!$J$2:$J$7</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">' 9.1B - 3'!$L$4</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!$L$4</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">' 9.1B - 3'!$L$6</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!$L$6</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">' 9.1B - 3'!#REF!</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!#REF!</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">' 9.1B - 3'!#REF!</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!#REF!</definedName>
     <definedName name="solver_rhs7" localSheetId="0" hidden="1">' 9.1B - 3'!$L$6</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!$L$6</definedName>
     <definedName name="solver_rhs8" localSheetId="0" hidden="1">' 9.1B - 3'!#REF!</definedName>
+    <definedName name="solver_rhs8" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!#REF!</definedName>
     <definedName name="solver_rhs9" localSheetId="0" hidden="1">' 9.1B - 3'!#REF!</definedName>
+    <definedName name="solver_rhs9" localSheetId="1" hidden="1">' 9.1B - 3 2.0'!#REF!</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -85,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="9">
   <si>
     <t>SOLVER</t>
   </si>
@@ -245,7 +304,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="2" tint="-0.24994659260841701"/>
@@ -549,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A36C73D-5DDD-4F70-818B-6E24CF2FC329}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,18 +997,572 @@
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="B2:G7 A8:H8">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+  <conditionalFormatting sqref="B2:G7 A8:I8">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:H19">
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:H11 A12:A16 B2:I2 I8 H3:I7">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+  <conditionalFormatting sqref="B2:I2 H3:I7 B11:H11 A12:A16">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DA6196-B8F0-4B0F-88A1-C02208E617E4}">
+  <dimension ref="A1:T21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="2">
+        <v>1</v>
+      </c>
+      <c r="P1" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>3</v>
+      </c>
+      <c r="R1" s="2">
+        <v>4</v>
+      </c>
+      <c r="S1" s="2">
+        <v>5</v>
+      </c>
+      <c r="T1" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <f t="array" ref="B2:G7">IF(TRANSPOSE(O2:T7) &lt;= 15,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6">
+        <f t="array" ref="H2:H7">MMULT(B2:G7,TRANSPOSE(B8:G8))</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" t="e">
+        <f ca="1">_xludf.MIN($J$8)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N2" s="8">
+        <v>1</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>14</v>
+      </c>
+      <c r="R2" s="3">
+        <v>18</v>
+      </c>
+      <c r="S2" s="3">
+        <v>10</v>
+      </c>
+      <c r="T2" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <f>COUNT($B$8:$G$8)</f>
+        <v>6</v>
+      </c>
+      <c r="L3" s="7"/>
+      <c r="N3" s="8">
+        <v>2</v>
+      </c>
+      <c r="O3" s="3">
+        <v>23</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>24</v>
+      </c>
+      <c r="R3" s="3">
+        <v>13</v>
+      </c>
+      <c r="S3" s="3">
+        <v>22</v>
+      </c>
+      <c r="T3" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <f t="array" ref="K4">($B$8:$G$8=0)+($B$8:$G$8=1)=1</f>
+        <v>1</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="N4" s="8">
+        <v>3</v>
+      </c>
+      <c r="O4" s="3">
+        <v>14</v>
+      </c>
+      <c r="P4" s="3">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3">
+        <v>60</v>
+      </c>
+      <c r="S4" s="3">
+        <v>19</v>
+      </c>
+      <c r="T4" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="K5" t="b">
+        <f t="array" ref="K5">$H$2:$H$7&gt;=$J$2:$J$7</f>
+        <v>1</v>
+      </c>
+      <c r="L5" s="7"/>
+      <c r="N5" s="8">
+        <v>4</v>
+      </c>
+      <c r="O5" s="3">
+        <v>18</v>
+      </c>
+      <c r="P5" s="3">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>60</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
+        <v>55</v>
+      </c>
+      <c r="T5" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <f>{32767;32767;0.000001;0.01;TRUE;FALSE;TRUE;1;1;1;0.0001;TRUE}</f>
+        <v>32767</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="N6" s="8">
+        <v>5</v>
+      </c>
+      <c r="O6" s="3">
+        <v>10</v>
+      </c>
+      <c r="P6" s="3">
+        <v>22</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>19</v>
+      </c>
+      <c r="R6" s="3">
+        <v>55</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0</v>
+      </c>
+      <c r="T6" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f>{0;0;2;100;0;FALSE;TRUE;0.075;0;0;FALSE;30}</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="8">
+        <v>6</v>
+      </c>
+      <c r="O7" s="3">
+        <v>32</v>
+      </c>
+      <c r="P7" s="3">
+        <v>11</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>20</v>
+      </c>
+      <c r="R7" s="3">
+        <v>17</v>
+      </c>
+      <c r="S7" s="3">
+        <v>12</v>
+      </c>
+      <c r="T7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4">
+        <f>SUM(B8:G8)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+    </row>
+    <row r="16" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:G7 A8:I8">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:H19">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:I2 H3:I7 B11:H11 A12:A16">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix: correção na 2.3E
</commit_message>
<xml_diff>
--- a/9.1B - 3.xlsx
+++ b/9.1B - 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Desktop\trabalhoPO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB45AF4-A493-4201-B0A9-005F5BCB11F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5197654-E6D6-4D8D-B483-6B4B21C391FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -177,7 +177,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +238,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -286,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -300,11 +316,28 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="2" tint="-0.24994659260841701"/>
@@ -998,17 +1031,17 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="B2:G7 A8:I8">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:H19">
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:I2 H3:I7 B11:H11 A12:A16">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1022,7 +1055,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,14 +1140,14 @@
       <c r="G2" s="6">
         <v>0</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="4">
         <f t="array" ref="H2:H7">MMULT(B2:G7,TRANSPOSE(B8:G8))</f>
         <v>1</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="10">
         <v>1</v>
       </c>
       <c r="K2" t="e">
@@ -1165,13 +1198,13 @@
       <c r="G3" s="3">
         <v>1</v>
       </c>
-      <c r="H3" s="6">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="10">
         <v>1</v>
       </c>
       <c r="K3">
@@ -1223,13 +1256,13 @@
       <c r="G4" s="3">
         <v>0</v>
       </c>
-      <c r="H4" s="6">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="10">
         <v>1</v>
       </c>
       <c r="K4" t="b">
@@ -1281,13 +1314,13 @@
       <c r="G5" s="3">
         <v>0</v>
       </c>
-      <c r="H5" s="6">
-        <v>1</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="10">
         <v>1</v>
       </c>
       <c r="K5" t="b">
@@ -1339,13 +1372,13 @@
       <c r="G6" s="3">
         <v>1</v>
       </c>
-      <c r="H6" s="6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="6" t="s">
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="10">
         <v>1</v>
       </c>
       <c r="K6">
@@ -1397,13 +1430,13 @@
       <c r="G7" s="3">
         <v>1</v>
       </c>
-      <c r="H7" s="6">
-        <v>1</v>
-      </c>
-      <c r="I7" s="6" t="s">
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="10">
         <v>1</v>
       </c>
       <c r="K7">
@@ -1453,10 +1486,10 @@
         <v>0</v>
       </c>
       <c r="H8" s="3"/>
-      <c r="I8" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="I8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="10">
         <f>SUM(B8:G8)</f>
         <v>2</v>
       </c>
@@ -1551,18 +1584,28 @@
       <c r="A21" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:G7 A8:I8">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="B17:H19">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:H19">
+  <conditionalFormatting sqref="B11:H11 A12:A16">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:G7 A8:I8">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:I2 H3:I7">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:I2 H3:I7 B11:H11 A12:A16">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  <conditionalFormatting sqref="O2:T7">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>